<commit_message>
After running up-to-date data" git status clear
</commit_message>
<xml_diff>
--- a/source/tab/originais/pop 1996 a 2022.xlsx
+++ b/source/tab/originais/pop 1996 a 2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\augustogeog\development\playground\projeção populacional\source\tab\originais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\augustogeog\development\playground\geodemography\source\tab\originais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E4CFCC-08B5-4EF8-9776-85C8A8DADE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83BC851-5606-479C-ABB4-CBD97581D70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB50EE22-3A68-486E-A891-A68D6DE63822}"/>
   </bookViews>
@@ -170,9 +170,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -210,7 +210,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -316,7 +316,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -458,7 +458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -468,7 +468,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FA5A69-869B-4812-A798-75EEA7660901}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -476,6 +478,7 @@
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -515,7 +518,7 @@
         <v>21664</v>
       </c>
       <c r="F2" s="3">
-        <v>22722.1</v>
+        <v>18157</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -535,7 +538,7 @@
         <v>88000</v>
       </c>
       <c r="F3" s="3">
-        <v>96867.9</v>
+        <v>80782</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -555,7 +558,7 @@
         <v>114907</v>
       </c>
       <c r="F4">
-        <v>117868</v>
+        <v>114101</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -575,7 +578,7 @@
         <v>133976</v>
       </c>
       <c r="F5">
-        <v>114922</v>
+        <v>112566</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -595,7 +598,7 @@
         <v>136653</v>
       </c>
       <c r="F6">
-        <v>123448</v>
+        <v>115697</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -615,7 +618,7 @@
         <v>295686</v>
       </c>
       <c r="F7" s="3">
-        <v>281189</v>
+        <v>278572</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -635,7 +638,7 @@
         <v>273849</v>
       </c>
       <c r="F8">
-        <v>280637</v>
+        <v>293800</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -655,7 +658,7 @@
         <v>235034</v>
       </c>
       <c r="F9">
-        <v>267790</v>
+        <v>281965</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -675,7 +678,7 @@
         <v>174535</v>
       </c>
       <c r="F10">
-        <v>223819</v>
+        <v>234356</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -695,7 +698,7 @@
         <v>100513</v>
       </c>
       <c r="F11">
-        <v>166719</v>
+        <v>174706</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -715,7 +718,7 @@
         <v>54159</v>
       </c>
       <c r="F12">
-        <v>92599</v>
+        <v>93580</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -735,7 +738,7 @@
         <v>25646</v>
       </c>
       <c r="F13">
-        <v>46127</v>
+        <v>43971</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -755,7 +758,7 @@
         <v>23357</v>
       </c>
       <c r="F14" s="3">
-        <v>23838.73</v>
+        <v>18488</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -775,7 +778,7 @@
         <v>90467</v>
       </c>
       <c r="F15" s="3">
-        <v>101628.27</v>
+        <v>83644</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -795,7 +798,7 @@
         <v>119374</v>
       </c>
       <c r="F16">
-        <v>123253</v>
+        <v>119030</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -815,7 +818,7 @@
         <v>139213</v>
       </c>
       <c r="F17">
-        <v>119212</v>
+        <v>117496</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -835,7 +838,7 @@
         <v>139069</v>
       </c>
       <c r="F18">
-        <v>128200</v>
+        <v>118852</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -855,7 +858,7 @@
         <v>291534</v>
       </c>
       <c r="F19" s="3">
-        <v>288490</v>
+        <v>278848</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -875,7 +878,7 @@
         <v>264132</v>
       </c>
       <c r="F20">
-        <v>270358</v>
+        <v>280289</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -895,7 +898,7 @@
         <v>214194</v>
       </c>
       <c r="F21">
-        <v>248253</v>
+        <v>261639</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -915,7 +918,7 @@
         <v>152041</v>
       </c>
       <c r="F22">
-        <v>196435</v>
+        <v>205547</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -935,7 +938,7 @@
         <v>83999</v>
       </c>
       <c r="F23">
-        <v>133034</v>
+        <v>140120</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -955,7 +958,7 @@
         <v>38374</v>
       </c>
       <c r="F24">
-        <v>66936</v>
+        <v>69260</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -975,7 +978,7 @@
         <v>13456</v>
       </c>
       <c r="F25">
-        <v>25020</v>
+        <v>24792</v>
       </c>
     </row>
   </sheetData>

</xml_diff>